<commit_message>
improved removal of bad characters in Identifiers
 A number of small changes to optimize the identifier formulate, the order of metadata attributes, the style of the version attribute, and the comments. Oh, and made the separation into sub-vocabularies prettier.
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niva/Documents/excel2rdf-template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Documents/GitHub/fair-data-collective/excel2rdf-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C87DFFBB-BC01-5E42-9009-948E7EEF62DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3696C76B-A976-4F46-BF6E-18D0F9958FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled-termilogy" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -123,12 +123,6 @@
     <t>Template for building SKOS based controlled vocabulary</t>
   </si>
   <si>
-    <t>This is a template for building SKOS based controlled vocabulary which is used as base of the worflow describe in excel2rdf.readthedocs.io/</t>
-  </si>
-  <si>
-    <t>TopConcetOne</t>
-  </si>
-  <si>
     <t>TopConceptTwo</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t>NarrowConceptTwo</t>
   </si>
   <si>
-    <t>temp-vocab:TopConcetOne</t>
-  </si>
-  <si>
     <t>temp-vocab:TopConceptTwo</t>
   </si>
   <si>
@@ -160,13 +151,43 @@
   </si>
   <si>
     <t>A definition of NarrowConceptTwo, which has a broader concept TopConceptTwo.</t>
+  </si>
+  <si>
+    <t>NarrowConceptThree</t>
+  </si>
+  <si>
+    <t>NarrowConceptFour</t>
+  </si>
+  <si>
+    <t>TopConceptOne</t>
+  </si>
+  <si>
+    <t>temp-vocab:TopConceptOne</t>
+  </si>
+  <si>
+    <t>Comments may be placed in this section of the spreadsheet, which can expand to fill more roles if need be. The converter will recognize where the Identifier line starts.</t>
+  </si>
+  <si>
+    <t>Best Concept</t>
+  </si>
+  <si>
+    <t>The user will need to extend the equation in column A down to include all the rows that are filled out.</t>
+  </si>
+  <si>
+    <t>0.1.0</t>
+  </si>
+  <si>
+    <t>This is a template for building a SKOS-based controlled vocabulary. It is used as base of the worflow described in excel2rdf.readthedocs.io/</t>
+  </si>
+  <si>
+    <t>The user will need to replace B1, B2-B3, and B5 through B12; B11 and B12 should be updated with every modification). (As well as these comments, if desired.)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -198,6 +219,10 @@
       <color rgb="FF0000FF"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -517,10 +542,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -599,7 +624,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -612,100 +637,91 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0.1</v>
+        <v>12</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I18" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="str">
-        <f t="shared" ref="A18:A19" si="0">"temp-vocab:"&amp;B18</f>
-        <v>temp-vocab:TopConcetOne</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>temp-vocab:TopConceptTwo</v>
+        <f>$B$2 &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B19," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
+        <v>temp-vocabTopConceptOne</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10" t="s">
@@ -715,90 +731,127 @@
         <v>26</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="str">
-        <f>"temp-vocab:"&amp;B20</f>
-        <v>temp-vocab:NarrowConceptOne</v>
+        <f t="shared" ref="A20:A24" si="0">$B$2 &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B20," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
+        <v>temp-vocabNarrowConceptOne</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="12"/>
+        <v>33</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E20" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="12"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="str">
-        <f t="shared" ref="A21" si="1">"temp-vocab:"&amp;B21</f>
-        <v>temp-vocab:NarrowConceptTwo</v>
+        <f t="shared" si="0"/>
+        <v>temp-vocabNarrowConceptTwo</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>temp-vocabTopConceptTwo</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H22" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>temp-vocabNarrowConceptThree</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="I23" s="12"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>temp-vocabNarrowConceptFour</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
+      <c r="D24" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="F24" s="11"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
+      <c r="G24" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="12"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
@@ -806,7 +859,7 @@
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
       <c r="E25" s="12"/>
-      <c r="F25" s="11"/>
+      <c r="F25" s="12"/>
       <c r="G25" s="13"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
@@ -916,7 +969,7 @@
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="12"/>
-      <c r="F35" s="14"/>
+      <c r="F35" s="11"/>
       <c r="G35" s="13"/>
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
@@ -927,17 +980,30 @@
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
       <c r="E36" s="12"/>
-      <c r="F36" s="11"/>
+      <c r="F36" s="14"/>
       <c r="G36" s="13"/>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
     </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="http://www.fair-data-collective.com/datasetvoc/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="C2" r:id="rId3" display="http://www.fair-data-collective.com/datasetvoc/" xr:uid="{B2511A53-6665-404C-95E0-E739BE247276}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
oops, fixed missing colons
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Documents/GitHub/fair-data-collective/excel2rdf-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3696C76B-A976-4F46-BF6E-18D0F9958FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52544DFE-C63D-7948-A7D5-536EF20BAE8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="controlled-termilogy" sheetId="1" r:id="rId1"/>
+    <sheet name="controlled-terminology" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -168,9 +168,6 @@
     <t>Comments may be placed in this section of the spreadsheet, which can expand to fill more roles if need be. The converter will recognize where the Identifier line starts.</t>
   </si>
   <si>
-    <t>Best Concept</t>
-  </si>
-  <si>
     <t>The user will need to extend the equation in column A down to include all the rows that are filled out.</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>The user will need to replace B1, B2-B3, and B5 through B12; B11 and B12 should be updated with every modification). (As well as these comments, if desired.)</t>
+  </si>
+  <si>
+    <t>Best Top Concept</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -562,7 +562,7 @@
     <col min="10" max="16384" width="11.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +570,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -581,7 +581,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -592,7 +592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -603,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -611,7 +611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -619,15 +619,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -635,7 +635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -651,7 +651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -659,12 +659,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -674,15 +674,15 @@
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
@@ -711,15 +711,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="str">
-        <f>$B$2 &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B19," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
-        <v>temp-vocabTopConceptOne</v>
+        <f>$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B19," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
+        <v>temp-vocab:TopConceptOne</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="D19" s="10" t="s">
         <v>31</v>
       </c>
@@ -737,15 +739,13 @@
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="str">
-        <f t="shared" ref="A20:A24" si="0">$B$2 &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B20," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
-        <v>temp-vocabNarrowConceptOne</v>
+        <f t="shared" ref="A20:A24" si="0">$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B20," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-"))</f>
+        <v>temp-vocab:NarrowConceptOne</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>45</v>
-      </c>
+      <c r="C20" s="11"/>
       <c r="D20" s="12" t="s">
         <v>38</v>
       </c>
@@ -762,7 +762,7 @@
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>temp-vocabNarrowConceptTwo</v>
+        <v>temp-vocab:NarrowConceptTwo</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>34</v>
@@ -781,10 +781,10 @@
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>temp-vocabTopConceptTwo</v>
+        <v>temp-vocab:TopConceptTwo</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>30</v>
@@ -805,10 +805,10 @@
       </c>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>temp-vocabNarrowConceptThree</v>
+        <v>temp-vocab:NarrowConceptThree</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>40</v>
@@ -829,10 +829,10 @@
       </c>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>temp-vocabNarrowConceptFour</v>
+        <v>temp-vocab:NarrowConceptFour</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>41</v>
@@ -853,7 +853,7 @@
       </c>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -864,7 +864,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -875,7 +875,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -886,7 +886,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -897,7 +897,7 @@
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -908,7 +908,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -919,7 +919,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -930,7 +930,7 @@
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -941,7 +941,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -952,7 +952,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -963,7 +963,7 @@
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -974,7 +974,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -985,7 +985,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>

</xml_diff>

<commit_message>
fixed the Identifier row (can't change it, oops!)
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Documents/GitHub/excel2rdf-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D84521-722F-3F4F-92C5-681807A29D05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F56E0B-6DE9-6C4F-8739-BAA3C713FB97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -78,6 +78,9 @@
     <t>pav:lastUpdatedOn</t>
   </si>
   <si>
+    <t>Identifier</t>
+  </si>
+  <si>
     <t>skos:prefLabel@en</t>
   </si>
   <si>
@@ -177,41 +180,20 @@
     <t>2021-02-20T15:54:00-08:00</t>
   </si>
   <si>
-    <r>
-      <t>Identifier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t>(autopopulated from column B)</t>
-    </r>
-  </si>
-  <si>
     <t>Replace cells B1, B2 and C2, and B5 through B12; B11 and B12 should be updated with every modification). (As well as these comments, if desired.)</t>
   </si>
   <si>
     <t>Extend the equation in column A down to include all the rows that are filled out. Verify that any special characters in the prefLabel are replaced by hyphens or other IRI-compatible ASCII characters.</t>
+  </si>
+  <si>
+    <t>In this spreadsheet, the identifier column gets filled out automatcially from the skos:prefLabel column. You can choose to replace any of the auto-generated identifiers.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -247,12 +229,6 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -585,18 +561,18 @@
   </sheetPr>
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="45.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="67.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="27.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="34.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="32.28515625" style="3" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" style="3" customWidth="1"/>
     <col min="9" max="9" width="22.140625" style="3" customWidth="1"/>
@@ -608,7 +584,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -616,10 +592,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -649,7 +625,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -657,7 +633,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -665,7 +641,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -678,10 +654,10 @@
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -697,7 +673,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -705,12 +681,12 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -723,33 +699,38 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -758,21 +739,21 @@
         <v>temp-vocab:TopConceptOne</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I21" s="8"/>
     </row>
@@ -782,18 +763,18 @@
         <v>temp-vocab:NarrowConceptOne</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -804,18 +785,18 @@
         <v>temp-vocab:NarrowConceptTwo</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
@@ -826,21 +807,21 @@
         <v>temp-vocab:TopConceptTwo</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I24" s="8"/>
     </row>
@@ -850,21 +831,21 @@
         <v>temp-vocab:NarrowConceptThree</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I25" s="10"/>
     </row>
@@ -874,21 +855,21 @@
         <v>temp-vocab:NarrowConceptFour</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I26" s="10"/>
     </row>

</xml_diff>